<commit_message>
[FEAT] Gives administrator full access to functions
</commit_message>
<xml_diff>
--- a/config_files/Horarios/Palobiofarma, S.L Mataró/Alina Ariosa.xlsx
+++ b/config_files/Horarios/Palobiofarma, S.L Mataró/Alina Ariosa.xlsx
@@ -7368,36 +7368,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="true"/>
-    <col min="2" max="2" width="6.77734375" customWidth="true"/>
-    <col min="3" max="3" width="6.77734375" customWidth="true"/>
-    <col min="4" max="4" width="6.77734375" customWidth="true"/>
-    <col min="5" max="5" width="6.77734375" customWidth="true"/>
-    <col min="6" max="6" width="6.77734375" customWidth="true"/>
-    <col min="7" max="7" width="6.77734375" customWidth="true"/>
-    <col min="8" max="8" width="6.77734375" customWidth="true"/>
-    <col min="9" max="9" width="2.77734375" customWidth="true"/>
-    <col min="10" max="10" width="6.77734375" customWidth="true"/>
-    <col min="11" max="11" width="6.77734375" customWidth="true"/>
-    <col min="12" max="12" width="6.77734375" customWidth="true"/>
-    <col min="13" max="13" width="6.77734375" customWidth="true"/>
-    <col min="14" max="14" width="6.77734375" customWidth="true"/>
-    <col min="15" max="15" width="6.77734375" customWidth="true"/>
-    <col min="16" max="16" width="6.77734375" customWidth="true"/>
-    <col min="17" max="17" width="2.77734375" customWidth="true"/>
-    <col min="18" max="18" width="6.77734375" customWidth="true"/>
-    <col min="19" max="19" width="6.77734375" customWidth="true"/>
-    <col min="20" max="20" width="6.77734375" customWidth="true"/>
-    <col min="21" max="21" width="6.77734375" customWidth="true"/>
-    <col min="22" max="22" width="6.77734375" customWidth="true"/>
-    <col min="23" max="23" width="6.77734375" customWidth="true"/>
-    <col min="24" max="24" width="6.77734375" customWidth="true"/>
-    <col min="25" max="25" width="10.0" customWidth="true"/>
-    <col min="26" max="26" width="6.0" customWidth="true"/>
-    <col min="27" max="27" width="21.77734375" customWidth="true"/>
-    <col min="28" max="28" width="21.77734375" customWidth="true"/>
-    <col min="29" max="29" width="21.77734375" customWidth="true"/>
-    <col min="30" max="30" width="10.0" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="2.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="2.77734375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="2.77734375" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="21.77734375" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="21.77734375" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="21.77734375" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.8" customHeight="true">
@@ -9399,23 +9399,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -9995,23 +9995,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -10598,23 +10598,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -11193,23 +11193,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -11795,23 +11795,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -12419,23 +12419,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -13028,23 +13028,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -13649,23 +13649,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -14261,23 +14261,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -14881,23 +14881,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -15479,23 +15479,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -16081,23 +16081,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">

</xml_diff>

<commit_message>
[FEAT] Added Updated Employee Pane
</commit_message>
<xml_diff>
--- a/config_files/Horarios/Palobiofarma, S.L Mataró/Alina Ariosa.xlsx
+++ b/config_files/Horarios/Palobiofarma, S.L Mataró/Alina Ariosa.xlsx
@@ -5703,7 +5703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="490">
+  <cellXfs count="491">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
     <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
@@ -6839,6 +6839,9 @@
     </xf>
     <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="489" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -7368,36 +7371,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="2.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="2.77734375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="2.77734375" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="6.77734375" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="21.77734375" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" width="21.77734375" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="21.77734375" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="2.77734375" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="2.77734375" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="2.77734375" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="20" max="20" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="21" max="21" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="22" max="22" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="23" max="23" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="24" max="24" customWidth="true" width="6.77734375" collapsed="false"/>
+    <col min="25" max="25" customWidth="true" width="10.0" collapsed="false"/>
+    <col min="26" max="26" customWidth="true" width="6.0" collapsed="false"/>
+    <col min="27" max="27" customWidth="true" width="21.77734375" collapsed="false"/>
+    <col min="28" max="28" customWidth="true" width="21.77734375" collapsed="false"/>
+    <col min="29" max="29" customWidth="true" width="21.77734375" collapsed="false"/>
+    <col min="30" max="30" customWidth="true" width="10.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.8" customHeight="true">
@@ -9399,23 +9402,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -9995,23 +9998,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -10598,23 +10601,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -11193,23 +11196,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -11795,23 +11798,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -11990,8 +11993,12 @@
       <c r="B18" s="127" t="n">
         <v>3.0</v>
       </c>
-      <c r="C18" s="128"/>
-      <c r="E18" s="128"/>
+      <c r="C18" s="490" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E18" s="490" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G18" s="125" t="n">
         <f>((E18-C18)*24)-1</f>
         <v>0.0</v>
@@ -12419,23 +12426,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -13028,23 +13035,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -13649,23 +13656,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -14261,23 +14268,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -14881,23 +14888,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -15479,23 +15486,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -16081,23 +16088,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">

</xml_diff>

<commit_message>
Added save button to Excel Table
</commit_message>
<xml_diff>
--- a/config_files/Horarios/Palobiofarma, S.L Mataró/Alina Ariosa.xlsx
+++ b/config_files/Horarios/Palobiofarma, S.L Mataró/Alina Ariosa.xlsx
@@ -5703,7 +5703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="497">
+  <cellXfs count="498">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
     <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
@@ -6839,6 +6839,9 @@
     </xf>
     <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="489" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment horizontal="center"/>
@@ -12003,10 +12006,10 @@
       <c r="B18" s="127" t="n">
         <v>3.0</v>
       </c>
-      <c r="C18" s="496" t="n">
+      <c r="C18" s="497" t="n">
         <v>0.3333333333333333</v>
       </c>
-      <c r="E18" s="496" t="n">
+      <c r="E18" s="497" t="n">
         <v>0.7083333333333334</v>
       </c>
       <c r="G18" s="125" t="n">
@@ -12018,10 +12021,10 @@
       <c r="B19" s="127" t="n">
         <v>4.0</v>
       </c>
-      <c r="C19" s="496" t="n">
+      <c r="C19" s="497" t="n">
         <v>0.375</v>
       </c>
-      <c r="E19" s="496" t="n">
+      <c r="E19" s="497" t="n">
         <v>0.7083333333333334</v>
       </c>
       <c r="G19" s="125" t="n">

</xml_diff>